<commit_message>
add gnuplot dat & esp
</commit_message>
<xml_diff>
--- a/exp_result/figure.xlsx
+++ b/exp_result/figure.xlsx
@@ -366,10 +366,6 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="11" numFmtId="165" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -400,6 +396,10 @@
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="13" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
@@ -478,7 +478,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart243.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart260.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2345,11 +2345,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="80764438"/>
-        <c:axId val="13331284"/>
+        <c:axId val="36073745"/>
+        <c:axId val="72471294"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="80764438"/>
+        <c:axId val="36073745"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2383,14 +2383,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="13331284"/>
+        <c:crossAx val="72471294"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="13331284"/>
+        <c:axId val="72471294"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2433,7 +2433,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="80764438"/>
+        <c:crossAx val="36073745"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2468,7 +2468,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart244.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart261.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3055,11 +3055,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="4878039"/>
-        <c:axId val="26714198"/>
+        <c:axId val="47435428"/>
+        <c:axId val="20902037"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="4878039"/>
+        <c:axId val="47435428"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3093,14 +3093,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="26714198"/>
+        <c:crossAx val="20902037"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="26714198"/>
+        <c:axId val="20902037"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3143,7 +3143,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="4878039"/>
+        <c:crossAx val="47435428"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -3178,7 +3178,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart245.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart262.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3765,11 +3765,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="74352891"/>
-        <c:axId val="75592885"/>
+        <c:axId val="32408391"/>
+        <c:axId val="2259538"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="74352891"/>
+        <c:axId val="32408391"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3803,14 +3803,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="75592885"/>
+        <c:crossAx val="2259538"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75592885"/>
+        <c:axId val="2259538"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3853,7 +3853,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="74352891"/>
+        <c:crossAx val="32408391"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -3888,7 +3888,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart246.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart263.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -5755,11 +5755,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="84828292"/>
-        <c:axId val="7420745"/>
+        <c:axId val="95042195"/>
+        <c:axId val="86175236"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84828292"/>
+        <c:axId val="95042195"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5793,14 +5793,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="7420745"/>
+        <c:crossAx val="86175236"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="7420745"/>
+        <c:axId val="86175236"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5843,7 +5843,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="84828292"/>
+        <c:crossAx val="95042195"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -5878,7 +5878,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart247.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart264.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -6465,11 +6465,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="54824110"/>
-        <c:axId val="74140158"/>
+        <c:axId val="74701296"/>
+        <c:axId val="47020556"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="54824110"/>
+        <c:axId val="74701296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6503,14 +6503,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="74140158"/>
+        <c:crossAx val="47020556"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74140158"/>
+        <c:axId val="47020556"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6553,7 +6553,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="54824110"/>
+        <c:crossAx val="74701296"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -6588,7 +6588,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart248.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart265.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -8455,11 +8455,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="53766845"/>
-        <c:axId val="19925406"/>
+        <c:axId val="79183206"/>
+        <c:axId val="12420651"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="53766845"/>
+        <c:axId val="79183206"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8493,14 +8493,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="19925406"/>
+        <c:crossAx val="12420651"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="19925406"/>
+        <c:axId val="12420651"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8543,7 +8543,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="53766845"/>
+        <c:crossAx val="79183206"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -8578,7 +8578,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart249.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart266.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -8798,11 +8798,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="99462009"/>
-        <c:axId val="40491618"/>
+        <c:axId val="98994108"/>
+        <c:axId val="81752836"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="99462009"/>
+        <c:axId val="98994108"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8836,14 +8836,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="40491618"/>
+        <c:crossAx val="81752836"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40491618"/>
+        <c:axId val="81752836"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8886,7 +8886,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="99462009"/>
+        <c:crossAx val="98994108"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -8921,7 +8921,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart250.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart267.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -9508,11 +9508,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="37719354"/>
-        <c:axId val="51973552"/>
+        <c:axId val="69328667"/>
+        <c:axId val="45475049"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="37719354"/>
+        <c:axId val="69328667"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9546,14 +9546,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="51973552"/>
+        <c:crossAx val="45475049"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51973552"/>
+        <c:axId val="45475049"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9596,7 +9596,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="37719354"/>
+        <c:crossAx val="69328667"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -9631,7 +9631,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart251.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart268.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -11498,11 +11498,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="2569629"/>
-        <c:axId val="4391664"/>
+        <c:axId val="8835786"/>
+        <c:axId val="87204942"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2569629"/>
+        <c:axId val="8835786"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11536,14 +11536,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="4391664"/>
+        <c:crossAx val="87204942"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="4391664"/>
+        <c:axId val="87204942"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11586,7 +11586,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2569629"/>
+        <c:crossAx val="8835786"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -11621,7 +11621,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart252.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart269.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -11841,11 +11841,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="93964589"/>
-        <c:axId val="27082950"/>
+        <c:axId val="27763752"/>
+        <c:axId val="43660823"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="93964589"/>
+        <c:axId val="27763752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11879,14 +11879,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="27082950"/>
+        <c:crossAx val="43660823"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="27082950"/>
+        <c:axId val="43660823"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11929,7 +11929,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="93964589"/>
+        <c:crossAx val="27763752"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -11964,7 +11964,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart253.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart270.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -12551,11 +12551,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="17876275"/>
-        <c:axId val="29772351"/>
+        <c:axId val="87512840"/>
+        <c:axId val="90033825"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="17876275"/>
+        <c:axId val="87512840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12589,14 +12589,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="29772351"/>
+        <c:crossAx val="90033825"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="29772351"/>
+        <c:axId val="90033825"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12639,7 +12639,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="17876275"/>
+        <c:crossAx val="87512840"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -12674,7 +12674,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart254.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart271.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -12894,11 +12894,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="82308685"/>
-        <c:axId val="47791546"/>
+        <c:axId val="33914823"/>
+        <c:axId val="23964585"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82308685"/>
+        <c:axId val="33914823"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12932,14 +12932,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="47791546"/>
+        <c:crossAx val="23964585"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47791546"/>
+        <c:axId val="23964585"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12982,7 +12982,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="82308685"/>
+        <c:crossAx val="33914823"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -13017,7 +13017,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart255.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart272.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -14884,11 +14884,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="62270073"/>
-        <c:axId val="37737648"/>
+        <c:axId val="90218351"/>
+        <c:axId val="9993580"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="62270073"/>
+        <c:axId val="90218351"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14922,14 +14922,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="37737648"/>
+        <c:crossAx val="9993580"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="37737648"/>
+        <c:axId val="9993580"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14972,7 +14972,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="62270073"/>
+        <c:crossAx val="90218351"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -15007,7 +15007,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart256.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart273.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -15337,11 +15337,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="83935393"/>
-        <c:axId val="184526"/>
+        <c:axId val="56235352"/>
+        <c:axId val="57182855"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="83935393"/>
+        <c:axId val="56235352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15357,14 +15357,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="184526"/>
+        <c:crossAx val="57182855"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="184526"/>
+        <c:axId val="57182855"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15389,7 +15389,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="83935393"/>
+        <c:crossAx val="56235352"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -15424,7 +15424,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart257.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart274.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -15754,11 +15754,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="23562404"/>
-        <c:axId val="32270767"/>
+        <c:axId val="19353127"/>
+        <c:axId val="54353756"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="23562404"/>
+        <c:axId val="19353127"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15774,14 +15774,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="32270767"/>
+        <c:crossAx val="54353756"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="32270767"/>
+        <c:axId val="54353756"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15806,7 +15806,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="23562404"/>
+        <c:crossAx val="19353127"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -15841,7 +15841,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart258.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart275.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -16171,11 +16171,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="14448152"/>
-        <c:axId val="56843195"/>
+        <c:axId val="29025399"/>
+        <c:axId val="55426872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="14448152"/>
+        <c:axId val="29025399"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16191,14 +16191,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="56843195"/>
+        <c:crossAx val="55426872"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="56843195"/>
+        <c:axId val="55426872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16223,7 +16223,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="14448152"/>
+        <c:crossAx val="29025399"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -16258,7 +16258,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart259.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart276.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -16588,11 +16588,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="98118403"/>
-        <c:axId val="71842543"/>
+        <c:axId val="79341402"/>
+        <c:axId val="76460827"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="98118403"/>
+        <c:axId val="79341402"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16608,14 +16608,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="71842543"/>
+        <c:crossAx val="76460827"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71842543"/>
+        <c:axId val="76460827"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16640,7 +16640,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="98118403"/>
+        <c:crossAx val="79341402"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -18521,7 +18521,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E9" activeCellId="0" pane="topLeft" sqref="E9"/>
+      <selection activeCell="F12" activeCellId="0" pane="topLeft" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24"/>
@@ -18605,7 +18605,7 @@
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="9" t="n">
+      <c r="B5" s="3" t="n">
         <v>72.1</v>
       </c>
       <c r="C5" s="3" t="n">
@@ -18625,7 +18625,7 @@
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="9" t="n">
+      <c r="B6" s="3" t="n">
         <v>518</v>
       </c>
       <c r="C6" s="3" t="n">
@@ -18751,19 +18751,19 @@
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="10" t="n">
+      <c r="B17" s="9" t="n">
         <v>610177390</v>
       </c>
-      <c r="C17" s="11" t="n">
+      <c r="C17" s="10" t="n">
         <v>129639608</v>
       </c>
-      <c r="D17" s="10" t="n">
+      <c r="D17" s="9" t="n">
         <v>370755163</v>
       </c>
-      <c r="E17" s="10" t="n">
+      <c r="E17" s="9" t="n">
         <v>200782497</v>
       </c>
-      <c r="F17" s="10" t="n">
+      <c r="F17" s="9" t="n">
         <v>129633747</v>
       </c>
     </row>
@@ -18771,19 +18771,19 @@
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="10" t="n">
+      <c r="B18" s="9" t="n">
         <v>596605140</v>
       </c>
-      <c r="C18" s="11" t="n">
+      <c r="C18" s="10" t="n">
         <v>86868777</v>
       </c>
-      <c r="D18" s="10" t="n">
+      <c r="D18" s="9" t="n">
         <v>235970840</v>
       </c>
-      <c r="E18" s="10" t="n">
+      <c r="E18" s="9" t="n">
         <v>198015767</v>
       </c>
-      <c r="F18" s="10" t="n">
+      <c r="F18" s="9" t="n">
         <v>86867884</v>
       </c>
     </row>
@@ -18791,19 +18791,19 @@
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="10" t="n">
+      <c r="B19" s="9" t="n">
         <v>589556446</v>
       </c>
-      <c r="C19" s="11" t="n">
+      <c r="C19" s="10" t="n">
         <v>139523979</v>
       </c>
-      <c r="D19" s="10" t="n">
+      <c r="D19" s="9" t="n">
         <v>585214921</v>
       </c>
-      <c r="E19" s="10" t="n">
+      <c r="E19" s="9" t="n">
         <v>201507491</v>
       </c>
-      <c r="F19" s="10" t="n">
+      <c r="F19" s="9" t="n">
         <v>139514355</v>
       </c>
     </row>
@@ -18811,19 +18811,19 @@
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="10" t="n">
+      <c r="B20" s="9" t="n">
         <v>632012049</v>
       </c>
-      <c r="C20" s="11" t="n">
+      <c r="C20" s="10" t="n">
         <v>87025191</v>
       </c>
-      <c r="D20" s="10" t="n">
+      <c r="D20" s="9" t="n">
         <v>243038014</v>
       </c>
-      <c r="E20" s="10" t="n">
+      <c r="E20" s="9" t="n">
         <v>200456553</v>
       </c>
-      <c r="F20" s="10" t="n">
+      <c r="F20" s="9" t="n">
         <v>87024279</v>
       </c>
     </row>
@@ -18831,19 +18831,19 @@
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="10" t="n">
+      <c r="B21" s="9" t="n">
         <v>556288257</v>
       </c>
-      <c r="C21" s="11" t="n">
+      <c r="C21" s="10" t="n">
         <v>453042555</v>
       </c>
-      <c r="D21" s="10" t="n">
+      <c r="D21" s="9" t="n">
         <v>565470664</v>
       </c>
-      <c r="E21" s="10" t="n">
+      <c r="E21" s="9" t="n">
         <v>201469456</v>
       </c>
-      <c r="F21" s="10" t="n">
+      <c r="F21" s="9" t="n">
         <v>452660678</v>
       </c>
     </row>
@@ -18851,19 +18851,19 @@
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="10" t="n">
+      <c r="B22" s="9" t="n">
         <v>639275393</v>
       </c>
-      <c r="C22" s="11" t="n">
+      <c r="C22" s="10" t="n">
         <v>386922465</v>
       </c>
-      <c r="D22" s="10" t="n">
+      <c r="D22" s="9" t="n">
         <v>195737997</v>
       </c>
-      <c r="E22" s="10" t="n">
+      <c r="E22" s="9" t="n">
         <v>199650829</v>
       </c>
-      <c r="F22" s="10" t="n">
+      <c r="F22" s="9" t="n">
         <v>385800474</v>
       </c>
     </row>
@@ -18871,19 +18871,19 @@
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="10" t="n">
+      <c r="B23" s="9" t="n">
         <v>803191351</v>
       </c>
-      <c r="C23" s="11" t="n">
+      <c r="C23" s="10" t="n">
         <v>113328330</v>
       </c>
-      <c r="D23" s="10" t="n">
+      <c r="D23" s="9" t="n">
         <v>474799118</v>
       </c>
-      <c r="E23" s="10" t="n">
+      <c r="E23" s="9" t="n">
         <v>199548453</v>
       </c>
-      <c r="F23" s="10" t="n">
+      <c r="F23" s="9" t="n">
         <v>113323833</v>
       </c>
     </row>
@@ -18891,19 +18891,19 @@
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="10" t="n">
+      <c r="B24" s="9" t="n">
         <v>612324367</v>
       </c>
-      <c r="C24" s="11" t="n">
+      <c r="C24" s="10" t="n">
         <v>413461554</v>
       </c>
-      <c r="D24" s="10" t="n">
+      <c r="D24" s="9" t="n">
         <v>568274521</v>
       </c>
-      <c r="E24" s="10" t="n">
+      <c r="E24" s="9" t="n">
         <v>200593583</v>
       </c>
-      <c r="F24" s="10" t="n">
+      <c r="F24" s="9" t="n">
         <v>412333863</v>
       </c>
     </row>
@@ -18911,19 +18911,19 @@
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="10" t="n">
+      <c r="B25" s="9" t="n">
         <v>766398717</v>
       </c>
-      <c r="C25" s="11" t="n">
+      <c r="C25" s="10" t="n">
         <v>86789429</v>
       </c>
-      <c r="D25" s="10" t="n">
+      <c r="D25" s="9" t="n">
         <v>258974976</v>
       </c>
-      <c r="E25" s="10" t="n">
+      <c r="E25" s="9" t="n">
         <v>201612541</v>
       </c>
-      <c r="F25" s="10" t="n">
+      <c r="F25" s="9" t="n">
         <v>86788476</v>
       </c>
     </row>
@@ -18931,19 +18931,19 @@
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="10" t="n">
+      <c r="B26" s="9" t="n">
         <v>613764095</v>
       </c>
-      <c r="C26" s="11" t="n">
+      <c r="C26" s="10" t="n">
         <v>131481872</v>
       </c>
-      <c r="D26" s="10" t="n">
+      <c r="D26" s="9" t="n">
         <v>608450334</v>
       </c>
-      <c r="E26" s="10" t="n">
+      <c r="E26" s="9" t="n">
         <v>198056126</v>
       </c>
-      <c r="F26" s="10" t="n">
+      <c r="F26" s="9" t="n">
         <v>131475850</v>
       </c>
     </row>
@@ -18951,19 +18951,19 @@
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="10" t="n">
+      <c r="B27" s="9" t="n">
         <v>661443671</v>
       </c>
-      <c r="C27" s="11" t="n">
+      <c r="C27" s="10" t="n">
         <v>80222339</v>
       </c>
-      <c r="D27" s="10" t="n">
+      <c r="D27" s="9" t="n">
         <v>267916338</v>
       </c>
-      <c r="E27" s="10" t="n">
+      <c r="E27" s="9" t="n">
         <v>198055850</v>
       </c>
-      <c r="F27" s="10" t="n">
+      <c r="F27" s="9" t="n">
         <v>80221601</v>
       </c>
     </row>
@@ -18971,19 +18971,19 @@
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="10" t="n">
+      <c r="B28" s="9" t="n">
         <v>589596394</v>
       </c>
-      <c r="C28" s="11" t="n">
+      <c r="C28" s="10" t="n">
         <v>142957255</v>
       </c>
-      <c r="D28" s="10" t="n">
+      <c r="D28" s="9" t="n">
         <v>478322952</v>
       </c>
-      <c r="E28" s="10" t="n">
+      <c r="E28" s="9" t="n">
         <v>196569888</v>
       </c>
-      <c r="F28" s="10" t="n">
+      <c r="F28" s="9" t="n">
         <v>142946573</v>
       </c>
     </row>
@@ -18991,19 +18991,19 @@
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="10" t="n">
+      <c r="B29" s="9" t="n">
         <v>609820455</v>
       </c>
-      <c r="C29" s="11" t="n">
+      <c r="C29" s="10" t="n">
         <v>80324073</v>
       </c>
-      <c r="D29" s="10" t="n">
+      <c r="D29" s="9" t="n">
         <v>245578441</v>
       </c>
-      <c r="E29" s="10" t="n">
+      <c r="E29" s="9" t="n">
         <v>202943871</v>
       </c>
-      <c r="F29" s="10" t="n">
+      <c r="F29" s="9" t="n">
         <v>80323343</v>
       </c>
     </row>
@@ -19011,19 +19011,19 @@
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="10" t="n">
+      <c r="B30" s="9" t="n">
         <v>609660712</v>
       </c>
-      <c r="C30" s="11" t="n">
+      <c r="C30" s="10" t="n">
         <v>466199747</v>
       </c>
-      <c r="D30" s="10" t="n">
+      <c r="D30" s="9" t="n">
         <v>625873334</v>
       </c>
-      <c r="E30" s="10" t="n">
+      <c r="E30" s="9" t="n">
         <v>200798845</v>
       </c>
-      <c r="F30" s="10" t="n">
+      <c r="F30" s="9" t="n">
         <v>465812831</v>
       </c>
     </row>
@@ -19031,19 +19031,19 @@
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="10" t="n">
+      <c r="B31" s="9" t="n">
         <v>601750729</v>
       </c>
-      <c r="C31" s="11" t="n">
+      <c r="C31" s="10" t="n">
         <v>86892928</v>
       </c>
-      <c r="D31" s="10" t="n">
+      <c r="D31" s="9" t="n">
         <v>212313256</v>
       </c>
-      <c r="E31" s="10" t="n">
+      <c r="E31" s="9" t="n">
         <v>199569002</v>
       </c>
-      <c r="F31" s="10" t="n">
+      <c r="F31" s="9" t="n">
         <v>86892014</v>
       </c>
     </row>
@@ -19051,19 +19051,19 @@
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="10" t="n">
+      <c r="B32" s="9" t="n">
         <v>748384539</v>
       </c>
-      <c r="C32" s="11" t="n">
+      <c r="C32" s="10" t="n">
         <v>413239153</v>
       </c>
-      <c r="D32" s="10" t="n">
+      <c r="D32" s="9" t="n">
         <v>585734298</v>
       </c>
-      <c r="E32" s="10" t="n">
+      <c r="E32" s="9" t="n">
         <v>198241482</v>
       </c>
-      <c r="F32" s="10" t="n">
+      <c r="F32" s="9" t="n">
         <v>412861323</v>
       </c>
     </row>
@@ -19071,19 +19071,19 @@
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="10" t="n">
+      <c r="B33" s="9" t="n">
         <v>669853633</v>
       </c>
-      <c r="C33" s="11" t="n">
+      <c r="C33" s="10" t="n">
         <v>420166436</v>
       </c>
-      <c r="D33" s="10" t="n">
+      <c r="D33" s="9" t="n">
         <v>236873689</v>
       </c>
-      <c r="E33" s="10" t="n">
+      <c r="E33" s="9" t="n">
         <v>200905005</v>
       </c>
-      <c r="F33" s="10" t="n">
+      <c r="F33" s="9" t="n">
         <v>419039047</v>
       </c>
     </row>
@@ -19091,19 +19091,19 @@
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="10" t="n">
+      <c r="B34" s="9" t="n">
         <v>881363303</v>
       </c>
-      <c r="C34" s="11" t="n">
+      <c r="C34" s="10" t="n">
         <v>71688535</v>
       </c>
-      <c r="D34" s="10" t="n">
+      <c r="D34" s="9" t="n">
         <v>394225005</v>
       </c>
-      <c r="E34" s="10" t="n">
+      <c r="E34" s="9" t="n">
         <v>199121799</v>
       </c>
-      <c r="F34" s="10" t="n">
+      <c r="F34" s="9" t="n">
         <v>71687994</v>
       </c>
     </row>
@@ -19111,19 +19111,19 @@
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="10" t="n">
+      <c r="B35" s="9" t="n">
         <v>616652515</v>
       </c>
-      <c r="C35" s="11" t="n">
+      <c r="C35" s="10" t="n">
         <v>131665130</v>
       </c>
-      <c r="D35" s="10" t="n">
+      <c r="D35" s="9" t="n">
         <v>582761821</v>
       </c>
-      <c r="E35" s="10" t="n">
+      <c r="E35" s="9" t="n">
         <v>199675385</v>
       </c>
-      <c r="F35" s="10" t="n">
+      <c r="F35" s="9" t="n">
         <v>131659078</v>
       </c>
     </row>
@@ -19131,19 +19131,19 @@
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="10" t="n">
+      <c r="B36" s="9" t="n">
         <v>721462100</v>
       </c>
-      <c r="C36" s="11" t="n">
+      <c r="C36" s="10" t="n">
         <v>78558063</v>
       </c>
-      <c r="D36" s="10" t="n">
+      <c r="D36" s="9" t="n">
         <v>263705850</v>
       </c>
-      <c r="E36" s="10" t="n">
+      <c r="E36" s="9" t="n">
         <v>202410341</v>
       </c>
-      <c r="F36" s="10" t="n">
+      <c r="F36" s="9" t="n">
         <v>78557409</v>
       </c>
     </row>
@@ -19178,12 +19178,12 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2212765957447"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1063829787234"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.4468085106383"/>
-    <col collapsed="false" hidden="false" max="256" min="7" style="12" width="10.1106382978723"/>
+    <col collapsed="false" hidden="false" max="256" min="7" style="11" width="10.1106382978723"/>
     <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.56595744680851"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="24" outlineLevel="0" r="1">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
     </row>
@@ -19288,12 +19288,12 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="24" outlineLevel="0" r="8">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="24" outlineLevel="0" r="9">
       <c r="A9" s="3" t="s">
@@ -19366,10 +19366,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="24" outlineLevel="0" r="15">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="11" t="s">
         <v>10</v>
       </c>
     </row>
@@ -19397,19 +19397,19 @@
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="14" t="n">
+      <c r="B17" s="13" t="n">
         <v>117638487</v>
       </c>
-      <c r="C17" s="15" t="n">
+      <c r="C17" s="14" t="n">
         <v>10123017</v>
       </c>
-      <c r="D17" s="16" t="n">
+      <c r="D17" s="15" t="n">
         <v>207099135</v>
       </c>
-      <c r="E17" s="16" t="n">
+      <c r="E17" s="15" t="n">
         <v>199126653</v>
       </c>
-      <c r="F17" s="16" t="n">
+      <c r="F17" s="15" t="n">
         <v>10123016</v>
       </c>
     </row>
@@ -19417,19 +19417,19 @@
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="16" t="n">
+      <c r="B18" s="15" t="n">
         <v>132840790</v>
       </c>
-      <c r="C18" s="15" t="n">
+      <c r="C18" s="14" t="n">
         <v>10247603</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="16" t="n">
+      <c r="E18" s="15" t="n">
         <v>199288073</v>
       </c>
-      <c r="F18" s="16" t="n">
+      <c r="F18" s="15" t="n">
         <v>10247601</v>
       </c>
     </row>
@@ -19437,19 +19437,19 @@
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="16" t="n">
+      <c r="B19" s="15" t="n">
         <v>119838342</v>
       </c>
-      <c r="C19" s="15" t="n">
+      <c r="C19" s="14" t="n">
         <v>10210255</v>
       </c>
-      <c r="D19" s="16" t="n">
+      <c r="D19" s="15" t="n">
         <v>212526355</v>
       </c>
-      <c r="E19" s="16" t="n">
+      <c r="E19" s="15" t="n">
         <v>199371413</v>
       </c>
-      <c r="F19" s="16" t="n">
+      <c r="F19" s="15" t="n">
         <v>10210255</v>
       </c>
     </row>
@@ -19457,19 +19457,19 @@
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="16" t="n">
+      <c r="B20" s="15" t="n">
         <v>150513176</v>
       </c>
-      <c r="C20" s="15" t="n">
+      <c r="C20" s="14" t="n">
         <v>10329974</v>
       </c>
-      <c r="D20" s="16" t="n">
+      <c r="D20" s="15" t="n">
         <v>159111680</v>
       </c>
-      <c r="E20" s="16" t="n">
+      <c r="E20" s="15" t="n">
         <v>201130293</v>
       </c>
-      <c r="F20" s="16" t="n">
+      <c r="F20" s="15" t="n">
         <v>10329973</v>
       </c>
     </row>
@@ -19477,19 +19477,19 @@
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="16" t="n">
+      <c r="B21" s="15" t="n">
         <v>115966768</v>
       </c>
-      <c r="C21" s="15" t="n">
+      <c r="C21" s="14" t="n">
         <v>1606799164</v>
       </c>
-      <c r="D21" s="16" t="n">
+      <c r="D21" s="15" t="n">
         <v>182746967</v>
       </c>
-      <c r="E21" s="16" t="n">
+      <c r="E21" s="15" t="n">
         <v>201047791</v>
       </c>
-      <c r="F21" s="16" t="n">
+      <c r="F21" s="15" t="n">
         <v>12206437</v>
       </c>
     </row>
@@ -19497,19 +19497,19 @@
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="16" t="n">
+      <c r="B22" s="15" t="n">
         <v>433191195</v>
       </c>
-      <c r="C22" s="15" t="n">
+      <c r="C22" s="14" t="n">
         <v>16978436</v>
       </c>
-      <c r="D22" s="16" t="n">
+      <c r="D22" s="15" t="n">
         <v>166685763</v>
       </c>
-      <c r="E22" s="16" t="n">
+      <c r="E22" s="15" t="n">
         <v>198959637</v>
       </c>
-      <c r="F22" s="16" t="n">
+      <c r="F22" s="15" t="n">
         <v>16976684</v>
       </c>
     </row>
@@ -19517,19 +19517,19 @@
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="16" t="n">
+      <c r="B23" s="15" t="n">
         <v>160335384</v>
       </c>
-      <c r="C23" s="15" t="n">
+      <c r="C23" s="14" t="n">
         <v>10208593</v>
       </c>
-      <c r="D23" s="16" t="n">
+      <c r="D23" s="15" t="n">
         <v>191359542</v>
       </c>
-      <c r="E23" s="16" t="n">
+      <c r="E23" s="15" t="n">
         <v>199876056</v>
       </c>
-      <c r="F23" s="16" t="n">
+      <c r="F23" s="15" t="n">
         <v>10208592</v>
       </c>
     </row>
@@ -19537,19 +19537,19 @@
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="16" t="n">
+      <c r="B24" s="15" t="n">
         <v>108301120</v>
       </c>
-      <c r="C24" s="15" t="n">
+      <c r="C24" s="14" t="n">
         <v>22987023</v>
       </c>
-      <c r="D24" s="16" t="n">
+      <c r="D24" s="15" t="n">
         <v>169673990</v>
       </c>
-      <c r="E24" s="16" t="n">
+      <c r="E24" s="15" t="n">
         <v>201050169</v>
       </c>
-      <c r="F24" s="16" t="n">
+      <c r="F24" s="15" t="n">
         <v>22954240</v>
       </c>
     </row>
@@ -19557,19 +19557,19 @@
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="16" t="n">
+      <c r="B25" s="15" t="n">
         <v>175086630</v>
       </c>
-      <c r="C25" s="15" t="n">
+      <c r="C25" s="14" t="n">
         <v>30299997</v>
       </c>
-      <c r="D25" s="16" t="n">
+      <c r="D25" s="15" t="n">
         <v>211150641</v>
       </c>
-      <c r="E25" s="16" t="n">
+      <c r="E25" s="15" t="n">
         <v>200614168</v>
       </c>
-      <c r="F25" s="16" t="n">
+      <c r="F25" s="15" t="n">
         <v>30297870</v>
       </c>
     </row>
@@ -19577,19 +19577,19 @@
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="16" t="n">
+      <c r="B26" s="15" t="n">
         <v>105033635</v>
       </c>
-      <c r="C26" s="15" t="n">
+      <c r="C26" s="14" t="n">
         <v>33787213</v>
       </c>
-      <c r="D26" s="16" t="n">
+      <c r="D26" s="15" t="n">
         <v>186080427</v>
       </c>
-      <c r="E26" s="16" t="n">
+      <c r="E26" s="15" t="n">
         <v>199486549</v>
       </c>
-      <c r="F26" s="16" t="n">
+      <c r="F26" s="15" t="n">
         <v>33773086</v>
       </c>
     </row>
@@ -19597,19 +19597,19 @@
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="16" t="n">
+      <c r="B27" s="15" t="n">
         <v>931231263</v>
       </c>
-      <c r="C27" s="15" t="n">
+      <c r="C27" s="14" t="n">
         <v>828514944</v>
       </c>
-      <c r="D27" s="16" t="n">
+      <c r="D27" s="15" t="n">
         <v>191903436</v>
       </c>
-      <c r="E27" s="16" t="n">
+      <c r="E27" s="15" t="n">
         <v>199102932</v>
       </c>
-      <c r="F27" s="16" t="n">
+      <c r="F27" s="15" t="n">
         <v>31216537</v>
       </c>
     </row>
@@ -19617,19 +19617,19 @@
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="16" t="n">
+      <c r="B28" s="15" t="n">
         <v>157665218</v>
       </c>
-      <c r="C28" s="15" t="n">
+      <c r="C28" s="14" t="n">
         <v>81361133</v>
       </c>
-      <c r="D28" s="16" t="n">
+      <c r="D28" s="15" t="n">
         <v>231903624</v>
       </c>
-      <c r="E28" s="16" t="n">
+      <c r="E28" s="15" t="n">
         <v>199324786</v>
       </c>
-      <c r="F28" s="16" t="n">
+      <c r="F28" s="15" t="n">
         <v>81293149</v>
       </c>
     </row>
@@ -19637,19 +19637,19 @@
       <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="16" t="n">
+      <c r="B29" s="15" t="n">
         <v>120801641</v>
       </c>
-      <c r="C29" s="15" t="n">
+      <c r="C29" s="14" t="n">
         <v>30125649</v>
       </c>
-      <c r="D29" s="16" t="n">
+      <c r="D29" s="15" t="n">
         <v>194417978</v>
       </c>
-      <c r="E29" s="16" t="n">
+      <c r="E29" s="15" t="n">
         <v>199321246</v>
       </c>
-      <c r="F29" s="16" t="n">
+      <c r="F29" s="15" t="n">
         <v>30123548</v>
       </c>
     </row>
@@ -19657,19 +19657,19 @@
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="16" t="n">
+      <c r="B30" s="15" t="n">
         <v>256547769</v>
       </c>
-      <c r="C30" s="15" t="n">
+      <c r="C30" s="14" t="n">
         <v>338881868</v>
       </c>
-      <c r="D30" s="16" t="n">
+      <c r="D30" s="15" t="n">
         <v>229687820</v>
       </c>
-      <c r="E30" s="16" t="n">
+      <c r="E30" s="15" t="n">
         <v>201175722</v>
       </c>
-      <c r="F30" s="16" t="n">
+      <c r="F30" s="15" t="n">
         <v>338573815</v>
       </c>
     </row>
@@ -19677,19 +19677,19 @@
       <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="16" t="n">
+      <c r="B31" s="15" t="n">
         <v>130335158</v>
       </c>
-      <c r="C31" s="15" t="n">
+      <c r="C31" s="14" t="n">
         <v>30122450</v>
       </c>
-      <c r="D31" s="16" t="n">
+      <c r="D31" s="15" t="n">
         <v>204385641</v>
       </c>
-      <c r="E31" s="16" t="n">
+      <c r="E31" s="15" t="n">
         <v>201066857</v>
       </c>
-      <c r="F31" s="16" t="n">
+      <c r="F31" s="15" t="n">
         <v>30120409</v>
       </c>
     </row>
@@ -19697,19 +19697,19 @@
       <c r="A32" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="16" t="n">
+      <c r="B32" s="15" t="n">
         <v>148617661</v>
       </c>
-      <c r="C32" s="15" t="n">
+      <c r="C32" s="14" t="n">
         <v>30024287</v>
       </c>
-      <c r="D32" s="16" t="n">
+      <c r="D32" s="15" t="n">
         <v>238559372</v>
       </c>
-      <c r="E32" s="16" t="n">
+      <c r="E32" s="15" t="n">
         <v>199090559</v>
       </c>
-      <c r="F32" s="16" t="n">
+      <c r="F32" s="15" t="n">
         <v>30022187</v>
       </c>
     </row>
@@ -19717,19 +19717,19 @@
       <c r="A33" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="16" t="n">
+      <c r="B33" s="15" t="n">
         <v>339858259</v>
       </c>
-      <c r="C33" s="15" t="n">
+      <c r="C33" s="14" t="n">
         <v>828425423</v>
       </c>
-      <c r="D33" s="16" t="n">
+      <c r="D33" s="15" t="n">
         <v>207432791</v>
       </c>
-      <c r="E33" s="16" t="n">
+      <c r="E33" s="15" t="n">
         <v>199292376</v>
       </c>
-      <c r="F33" s="16" t="n">
+      <c r="F33" s="15" t="n">
         <v>31126911</v>
       </c>
     </row>
@@ -19737,19 +19737,19 @@
       <c r="A34" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="16" t="n">
+      <c r="B34" s="15" t="n">
         <v>170647805</v>
       </c>
-      <c r="C34" s="15" t="n">
+      <c r="C34" s="14" t="n">
         <v>30187878</v>
       </c>
-      <c r="D34" s="16" t="n">
+      <c r="D34" s="15" t="n">
         <v>229145449</v>
       </c>
-      <c r="E34" s="16" t="n">
+      <c r="E34" s="15" t="n">
         <v>199351204</v>
       </c>
-      <c r="F34" s="16" t="n">
+      <c r="F34" s="15" t="n">
         <v>30185817</v>
       </c>
     </row>
@@ -19757,19 +19757,19 @@
       <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="16" t="n">
+      <c r="B35" s="15" t="n">
         <v>118565721</v>
       </c>
-      <c r="C35" s="15" t="n">
+      <c r="C35" s="14" t="n">
         <v>10041789</v>
       </c>
-      <c r="D35" s="16" t="n">
+      <c r="D35" s="15" t="n">
         <v>196857801</v>
       </c>
-      <c r="E35" s="16" t="n">
+      <c r="E35" s="15" t="n">
         <v>201184186</v>
       </c>
-      <c r="F35" s="16" t="n">
+      <c r="F35" s="15" t="n">
         <v>10041788</v>
       </c>
     </row>
@@ -19777,19 +19777,19 @@
       <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="16" t="n">
+      <c r="B36" s="15" t="n">
         <v>182291801</v>
       </c>
-      <c r="C36" s="15" t="n">
+      <c r="C36" s="14" t="n">
         <v>30339703</v>
       </c>
-      <c r="D36" s="16" t="n">
+      <c r="D36" s="15" t="n">
         <v>212827921</v>
       </c>
-      <c r="E36" s="16" t="n">
+      <c r="E36" s="15" t="n">
         <v>201123383</v>
       </c>
-      <c r="F36" s="16" t="n">
+      <c r="F36" s="15" t="n">
         <v>30337604</v>
       </c>
     </row>
@@ -19828,7 +19828,7 @@
     <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.56595744680851"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="24" outlineLevel="0" r="1" s="9">
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="24" outlineLevel="0" r="1" s="17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -19933,7 +19933,7 @@
         <v>226</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="24" outlineLevel="0" r="8" s="9">
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="24" outlineLevel="0" r="8" s="17">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -20011,11 +20011,11 @@
         <v>12.5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="24" outlineLevel="0" r="15" s="9">
-      <c r="A15" s="9" t="s">
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="24" outlineLevel="0" r="15" s="17">
+      <c r="A15" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="17" t="s">
         <v>10</v>
       </c>
     </row>
@@ -20043,19 +20043,19 @@
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="15" t="n">
+      <c r="B17" s="14" t="n">
         <v>118582663</v>
       </c>
-      <c r="C17" s="15" t="n">
+      <c r="C17" s="14" t="n">
         <v>10126189</v>
       </c>
-      <c r="D17" s="15" t="n">
+      <c r="D17" s="14" t="n">
         <v>117182547</v>
       </c>
-      <c r="E17" s="15" t="n">
+      <c r="E17" s="14" t="n">
         <v>200919452</v>
       </c>
-      <c r="F17" s="15" t="n">
+      <c r="F17" s="14" t="n">
         <v>10126188</v>
       </c>
     </row>
@@ -20063,19 +20063,19 @@
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="15" t="n">
+      <c r="B18" s="14" t="n">
         <v>134433075</v>
       </c>
-      <c r="C18" s="15" t="n">
+      <c r="C18" s="14" t="n">
         <v>10248428</v>
       </c>
-      <c r="D18" s="15" t="n">
+      <c r="D18" s="14" t="n">
         <v>10368995</v>
       </c>
-      <c r="E18" s="15" t="n">
+      <c r="E18" s="14" t="n">
         <v>199683640</v>
       </c>
-      <c r="F18" s="15" t="n">
+      <c r="F18" s="14" t="n">
         <v>10248428</v>
       </c>
     </row>
@@ -20083,19 +20083,19 @@
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="15" t="n">
+      <c r="B19" s="14" t="n">
         <v>120356840</v>
       </c>
-      <c r="C19" s="15" t="n">
+      <c r="C19" s="14" t="n">
         <v>10205107</v>
       </c>
-      <c r="D19" s="15" t="n">
+      <c r="D19" s="14" t="n">
         <v>61107370</v>
       </c>
-      <c r="E19" s="15" t="n">
+      <c r="E19" s="14" t="n">
         <v>201462559</v>
       </c>
-      <c r="F19" s="15" t="n">
+      <c r="F19" s="14" t="n">
         <v>10205105</v>
       </c>
     </row>
@@ -20103,19 +20103,19 @@
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="15" t="n">
+      <c r="B20" s="14" t="n">
         <v>154078494</v>
       </c>
-      <c r="C20" s="15" t="n">
+      <c r="C20" s="14" t="n">
         <v>10325903</v>
       </c>
-      <c r="D20" s="15" t="n">
+      <c r="D20" s="14" t="n">
         <v>30346388</v>
       </c>
-      <c r="E20" s="15" t="n">
+      <c r="E20" s="14" t="n">
         <v>199111109</v>
       </c>
-      <c r="F20" s="15" t="n">
+      <c r="F20" s="14" t="n">
         <v>10325902</v>
       </c>
     </row>
@@ -20123,19 +20123,19 @@
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="15" t="n">
+      <c r="B21" s="14" t="n">
         <v>117450618</v>
       </c>
-      <c r="C21" s="15" t="n">
+      <c r="C21" s="14" t="n">
         <v>1606813145</v>
       </c>
-      <c r="D21" s="15" t="n">
+      <c r="D21" s="14" t="n">
         <v>33432665</v>
       </c>
-      <c r="E21" s="15" t="n">
+      <c r="E21" s="14" t="n">
         <v>198814542</v>
       </c>
-      <c r="F21" s="15" t="n">
+      <c r="F21" s="14" t="n">
         <v>12212696</v>
       </c>
     </row>
@@ -20143,19 +20143,19 @@
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="15" t="n">
+      <c r="B22" s="14" t="n">
         <v>956833278</v>
       </c>
-      <c r="C22" s="15" t="n">
+      <c r="C22" s="14" t="n">
         <v>16965048</v>
       </c>
-      <c r="D22" s="15" t="n">
+      <c r="D22" s="14" t="n">
         <v>1626943113</v>
       </c>
-      <c r="E22" s="15" t="n">
+      <c r="E22" s="14" t="n">
         <v>199793674</v>
       </c>
-      <c r="F22" s="15" t="n">
+      <c r="F22" s="14" t="n">
         <v>16963509</v>
       </c>
     </row>
@@ -20163,19 +20163,19 @@
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="15" t="n">
+      <c r="B23" s="14" t="n">
         <v>167353645</v>
       </c>
-      <c r="C23" s="15" t="n">
+      <c r="C23" s="14" t="n">
         <v>10205210</v>
       </c>
-      <c r="D23" s="15" t="n">
+      <c r="D23" s="14" t="n">
         <v>22579693</v>
       </c>
-      <c r="E23" s="15" t="n">
+      <c r="E23" s="14" t="n">
         <v>201275806</v>
       </c>
-      <c r="F23" s="15" t="n">
+      <c r="F23" s="14" t="n">
         <v>10205207</v>
       </c>
     </row>
@@ -20183,19 +20183,19 @@
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="15" t="n">
+      <c r="B24" s="14" t="n">
         <v>108991567</v>
       </c>
-      <c r="C24" s="15" t="n">
+      <c r="C24" s="14" t="n">
         <v>22990586</v>
       </c>
-      <c r="D24" s="15" t="n">
+      <c r="D24" s="14" t="n">
         <v>30286171</v>
       </c>
-      <c r="E24" s="15" t="n">
+      <c r="E24" s="14" t="n">
         <v>199338518</v>
       </c>
-      <c r="F24" s="15" t="n">
+      <c r="F24" s="14" t="n">
         <v>22958835</v>
       </c>
     </row>
@@ -20203,19 +20203,19 @@
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="15" t="n">
+      <c r="B25" s="14" t="n">
         <v>177195683</v>
       </c>
-      <c r="C25" s="15" t="n">
+      <c r="C25" s="14" t="n">
         <v>30303259</v>
       </c>
-      <c r="D25" s="15" t="n">
+      <c r="D25" s="14" t="n">
         <v>16686231</v>
       </c>
-      <c r="E25" s="15" t="n">
+      <c r="E25" s="14" t="n">
         <v>198495152</v>
       </c>
-      <c r="F25" s="15" t="n">
+      <c r="F25" s="14" t="n">
         <v>30301481</v>
       </c>
     </row>
@@ -20223,19 +20223,19 @@
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="15" t="n">
+      <c r="B26" s="14" t="n">
         <v>105821977</v>
       </c>
-      <c r="C26" s="15" t="n">
+      <c r="C26" s="14" t="n">
         <v>33787917</v>
       </c>
-      <c r="D26" s="15" t="n">
+      <c r="D26" s="14" t="n">
         <v>30132667</v>
       </c>
-      <c r="E26" s="15" t="n">
+      <c r="E26" s="14" t="n">
         <v>201080670</v>
       </c>
-      <c r="F26" s="15" t="n">
+      <c r="F26" s="14" t="n">
         <v>33774243</v>
       </c>
     </row>
@@ -20243,19 +20243,19 @@
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="15" t="n">
+      <c r="B27" s="14" t="n">
         <v>964964182</v>
       </c>
-      <c r="C27" s="15" t="n">
+      <c r="C27" s="14" t="n">
         <v>828520283</v>
       </c>
-      <c r="D27" s="15" t="n">
+      <c r="D27" s="14" t="n">
         <v>30329186</v>
       </c>
-      <c r="E27" s="15" t="n">
+      <c r="E27" s="14" t="n">
         <v>200898560</v>
       </c>
-      <c r="F27" s="15" t="n">
+      <c r="F27" s="14" t="n">
         <v>31218362</v>
       </c>
     </row>
@@ -20263,19 +20263,19 @@
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="15" t="n">
+      <c r="B28" s="14" t="n">
         <v>165550290</v>
       </c>
-      <c r="C28" s="15" t="n">
+      <c r="C28" s="14" t="n">
         <v>81349074</v>
       </c>
-      <c r="D28" s="15" t="n">
+      <c r="D28" s="14" t="n">
         <v>828268037</v>
       </c>
-      <c r="E28" s="15" t="n">
+      <c r="E28" s="14" t="n">
         <v>199714803</v>
       </c>
-      <c r="F28" s="15" t="n">
+      <c r="F28" s="14" t="n">
         <v>81282420</v>
       </c>
     </row>
@@ -20283,19 +20283,19 @@
       <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="15" t="n">
+      <c r="B29" s="14" t="n">
         <v>121836238</v>
       </c>
-      <c r="C29" s="15" t="n">
+      <c r="C29" s="14" t="n">
         <v>30132773</v>
       </c>
-      <c r="D29" s="15" t="n">
+      <c r="D29" s="14" t="n">
         <v>30497900</v>
       </c>
-      <c r="E29" s="15" t="n">
+      <c r="E29" s="14" t="n">
         <v>201454643</v>
       </c>
-      <c r="F29" s="15" t="n">
+      <c r="F29" s="14" t="n">
         <v>30131027</v>
       </c>
     </row>
@@ -20303,19 +20303,19 @@
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="15" t="n">
+      <c r="B30" s="14" t="n">
         <v>266671929</v>
       </c>
-      <c r="C30" s="15" t="n">
+      <c r="C30" s="14" t="n">
         <v>338893684</v>
       </c>
-      <c r="D30" s="15" t="n">
+      <c r="D30" s="14" t="n">
         <v>10004289</v>
       </c>
-      <c r="E30" s="15" t="n">
+      <c r="E30" s="14" t="n">
         <v>199116753</v>
       </c>
-      <c r="F30" s="15" t="n">
+      <c r="F30" s="14" t="n">
         <v>338592708</v>
       </c>
     </row>
@@ -20323,19 +20323,19 @@
       <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="15" t="n">
+      <c r="B31" s="14" t="n">
         <v>131904682</v>
       </c>
-      <c r="C31" s="15" t="n">
+      <c r="C31" s="14" t="n">
         <v>30127389</v>
       </c>
-      <c r="D31" s="15" t="n">
+      <c r="D31" s="14" t="n">
         <v>30703274</v>
       </c>
-      <c r="E31" s="15" t="n">
+      <c r="E31" s="14" t="n">
         <v>198817526</v>
       </c>
-      <c r="F31" s="15" t="n">
+      <c r="F31" s="14" t="n">
         <v>30125599</v>
       </c>
     </row>
@@ -20343,19 +20343,19 @@
       <c r="A32" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="15" t="n">
+      <c r="B32" s="14" t="n">
         <v>149789031</v>
       </c>
-      <c r="C32" s="15" t="n">
+      <c r="C32" s="14" t="n">
         <v>30016983</v>
       </c>
-      <c r="D32" s="15" t="n">
+      <c r="D32" s="14" t="n">
         <v>10004830</v>
       </c>
-      <c r="E32" s="15" t="n">
+      <c r="E32" s="14" t="n">
         <v>200960014</v>
       </c>
-      <c r="F32" s="15" t="n">
+      <c r="F32" s="14" t="n">
         <v>30015165</v>
       </c>
     </row>
@@ -20363,19 +20363,19 @@
       <c r="A33" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="15" t="n">
+      <c r="B33" s="14" t="n">
         <v>346741688</v>
       </c>
-      <c r="C33" s="15" t="n">
+      <c r="C33" s="14" t="n">
         <v>828426078</v>
       </c>
-      <c r="D33" s="15" t="n">
+      <c r="D33" s="14" t="n">
         <v>232272280</v>
       </c>
-      <c r="E33" s="15" t="n">
+      <c r="E33" s="14" t="n">
         <v>199636589</v>
       </c>
-      <c r="F33" s="15" t="n">
+      <c r="F33" s="14" t="n">
         <v>31124177</v>
       </c>
     </row>
@@ -20383,19 +20383,19 @@
       <c r="A34" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="15" t="n">
+      <c r="B34" s="14" t="n">
         <v>171028004</v>
       </c>
-      <c r="C34" s="15" t="n">
+      <c r="C34" s="14" t="n">
         <v>30175628</v>
       </c>
-      <c r="D34" s="15" t="n">
+      <c r="D34" s="14" t="n">
         <v>808345115</v>
       </c>
-      <c r="E34" s="15" t="n">
+      <c r="E34" s="14" t="n">
         <v>201464941</v>
       </c>
-      <c r="F34" s="15" t="n">
+      <c r="F34" s="14" t="n">
         <v>30173780</v>
       </c>
     </row>
@@ -20403,19 +20403,19 @@
       <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="15" t="n">
+      <c r="B35" s="14" t="n">
         <v>119484573</v>
       </c>
-      <c r="C35" s="15" t="n">
+      <c r="C35" s="14" t="n">
         <v>10042177</v>
       </c>
-      <c r="D35" s="15" t="n">
+      <c r="D35" s="14" t="n">
         <v>30303424</v>
       </c>
-      <c r="E35" s="15" t="n">
+      <c r="E35" s="14" t="n">
         <v>199109475</v>
       </c>
-      <c r="F35" s="15" t="n">
+      <c r="F35" s="14" t="n">
         <v>10042177</v>
       </c>
     </row>
@@ -20423,19 +20423,19 @@
       <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="15" t="n">
+      <c r="B36" s="14" t="n">
         <v>181854606</v>
       </c>
-      <c r="C36" s="15" t="n">
+      <c r="C36" s="14" t="n">
         <v>30341308</v>
       </c>
-      <c r="D36" s="15" t="n">
+      <c r="D36" s="14" t="n">
         <v>10201929</v>
       </c>
-      <c r="E36" s="15" t="n">
+      <c r="E36" s="14" t="n">
         <v>198835860</v>
       </c>
-      <c r="F36" s="15" t="n">
+      <c r="F36" s="14" t="n">
         <v>30339475</v>
       </c>
     </row>
@@ -20489,7 +20489,7 @@
       <c r="B4" s="8" t="n">
         <v>85889982</v>
       </c>
-      <c r="C4" s="10" t="n">
+      <c r="C4" s="9" t="n">
         <v>200782497</v>
       </c>
     </row>
@@ -20500,7 +20500,7 @@
       <c r="B5" s="8" t="n">
         <v>86326753</v>
       </c>
-      <c r="C5" s="10" t="n">
+      <c r="C5" s="9" t="n">
         <v>198015767</v>
       </c>
     </row>
@@ -20511,7 +20511,7 @@
       <c r="B6" s="8" t="n">
         <v>92441831</v>
       </c>
-      <c r="C6" s="10" t="n">
+      <c r="C6" s="9" t="n">
         <v>201507491</v>
       </c>
     </row>
@@ -20522,7 +20522,7 @@
       <c r="B7" s="8" t="n">
         <v>88390618</v>
       </c>
-      <c r="C7" s="10" t="n">
+      <c r="C7" s="9" t="n">
         <v>200456553</v>
       </c>
     </row>
@@ -20533,7 +20533,7 @@
       <c r="B8" s="8" t="n">
         <v>87100621</v>
       </c>
-      <c r="C8" s="10" t="n">
+      <c r="C8" s="9" t="n">
         <v>201469456</v>
       </c>
     </row>
@@ -20544,7 +20544,7 @@
       <c r="B9" s="8" t="n">
         <v>45183323</v>
       </c>
-      <c r="C9" s="10" t="n">
+      <c r="C9" s="9" t="n">
         <v>199650829</v>
       </c>
     </row>
@@ -20555,7 +20555,7 @@
       <c r="B10" s="8" t="n">
         <v>48449880</v>
       </c>
-      <c r="C10" s="10" t="n">
+      <c r="C10" s="9" t="n">
         <v>199548453</v>
       </c>
     </row>
@@ -20566,7 +20566,7 @@
       <c r="B11" s="8" t="n">
         <v>53844429</v>
       </c>
-      <c r="C11" s="10" t="n">
+      <c r="C11" s="9" t="n">
         <v>200593583</v>
       </c>
     </row>
@@ -20577,7 +20577,7 @@
       <c r="B12" s="8" t="n">
         <v>59093945</v>
       </c>
-      <c r="C12" s="10" t="n">
+      <c r="C12" s="9" t="n">
         <v>201612541</v>
       </c>
     </row>
@@ -20588,7 +20588,7 @@
       <c r="B13" s="8" t="n">
         <v>57693136</v>
       </c>
-      <c r="C13" s="10" t="n">
+      <c r="C13" s="9" t="n">
         <v>198056126</v>
       </c>
     </row>
@@ -20599,7 +20599,7 @@
       <c r="B14" s="8" t="n">
         <v>73514007</v>
       </c>
-      <c r="C14" s="10" t="n">
+      <c r="C14" s="9" t="n">
         <v>198055850</v>
       </c>
     </row>
@@ -20610,7 +20610,7 @@
       <c r="B15" s="8" t="n">
         <v>78521475</v>
       </c>
-      <c r="C15" s="10" t="n">
+      <c r="C15" s="9" t="n">
         <v>196569888</v>
       </c>
     </row>
@@ -20621,7 +20621,7 @@
       <c r="B16" s="8" t="n">
         <v>75205826</v>
       </c>
-      <c r="C16" s="10" t="n">
+      <c r="C16" s="9" t="n">
         <v>202943871</v>
       </c>
     </row>
@@ -20632,7 +20632,7 @@
       <c r="B17" s="8" t="n">
         <v>71162646</v>
       </c>
-      <c r="C17" s="10" t="n">
+      <c r="C17" s="9" t="n">
         <v>200798845</v>
       </c>
     </row>
@@ -20643,7 +20643,7 @@
       <c r="B18" s="8" t="n">
         <v>75182142</v>
       </c>
-      <c r="C18" s="10" t="n">
+      <c r="C18" s="9" t="n">
         <v>199569002</v>
       </c>
     </row>
@@ -20654,7 +20654,7 @@
       <c r="B19" s="8" t="n">
         <v>55020266</v>
       </c>
-      <c r="C19" s="10" t="n">
+      <c r="C19" s="9" t="n">
         <v>198241482</v>
       </c>
     </row>
@@ -20665,7 +20665,7 @@
       <c r="B20" s="8" t="n">
         <v>54134706</v>
       </c>
-      <c r="C20" s="10" t="n">
+      <c r="C20" s="9" t="n">
         <v>200905005</v>
       </c>
     </row>
@@ -20676,7 +20676,7 @@
       <c r="B21" s="8" t="n">
         <v>57481333</v>
       </c>
-      <c r="C21" s="10" t="n">
+      <c r="C21" s="9" t="n">
         <v>199121799</v>
       </c>
     </row>
@@ -20687,7 +20687,7 @@
       <c r="B22" s="8" t="n">
         <v>48281837</v>
       </c>
-      <c r="C22" s="10" t="n">
+      <c r="C22" s="9" t="n">
         <v>199675385</v>
       </c>
     </row>
@@ -20698,7 +20698,7 @@
       <c r="B23" s="8" t="n">
         <v>54220285</v>
       </c>
-      <c r="C23" s="10" t="n">
+      <c r="C23" s="9" t="n">
         <v>202410341</v>
       </c>
     </row>
@@ -20720,7 +20720,7 @@
       <c r="B27" s="8" t="n">
         <v>81704694</v>
       </c>
-      <c r="C27" s="10" t="n">
+      <c r="C27" s="9" t="n">
         <v>610177390</v>
       </c>
     </row>
@@ -20731,7 +20731,7 @@
       <c r="B28" s="8" t="n">
         <v>81682814</v>
       </c>
-      <c r="C28" s="10" t="n">
+      <c r="C28" s="9" t="n">
         <v>596605140</v>
       </c>
     </row>
@@ -20742,7 +20742,7 @@
       <c r="B29" s="8" t="n">
         <v>82292433</v>
       </c>
-      <c r="C29" s="10" t="n">
+      <c r="C29" s="9" t="n">
         <v>589556446</v>
       </c>
     </row>
@@ -20753,7 +20753,7 @@
       <c r="B30" s="8" t="n">
         <v>81699600</v>
       </c>
-      <c r="C30" s="10" t="n">
+      <c r="C30" s="9" t="n">
         <v>632012049</v>
       </c>
     </row>
@@ -20764,7 +20764,7 @@
       <c r="B31" s="8" t="n">
         <v>81698058</v>
       </c>
-      <c r="C31" s="10" t="n">
+      <c r="C31" s="9" t="n">
         <v>556288257</v>
       </c>
     </row>
@@ -20775,7 +20775,7 @@
       <c r="B32" s="8" t="n">
         <v>81389270</v>
       </c>
-      <c r="C32" s="10" t="n">
+      <c r="C32" s="9" t="n">
         <v>639275393</v>
       </c>
     </row>
@@ -20786,7 +20786,7 @@
       <c r="B33" s="8" t="n">
         <v>81405851</v>
       </c>
-      <c r="C33" s="10" t="n">
+      <c r="C33" s="9" t="n">
         <v>803191351</v>
       </c>
     </row>
@@ -20797,7 +20797,7 @@
       <c r="B34" s="8" t="n">
         <v>82296064</v>
       </c>
-      <c r="C34" s="10" t="n">
+      <c r="C34" s="9" t="n">
         <v>612324367</v>
       </c>
     </row>
@@ -20808,7 +20808,7 @@
       <c r="B35" s="8" t="n">
         <v>82287728</v>
       </c>
-      <c r="C35" s="10" t="n">
+      <c r="C35" s="9" t="n">
         <v>766398717</v>
       </c>
     </row>
@@ -20819,7 +20819,7 @@
       <c r="B36" s="8" t="n">
         <v>81379534</v>
       </c>
-      <c r="C36" s="10" t="n">
+      <c r="C36" s="9" t="n">
         <v>613764095</v>
       </c>
     </row>
@@ -20830,7 +20830,7 @@
       <c r="B37" s="8" t="n">
         <v>82593135</v>
       </c>
-      <c r="C37" s="10" t="n">
+      <c r="C37" s="9" t="n">
         <v>661443671</v>
       </c>
     </row>
@@ -20841,7 +20841,7 @@
       <c r="B38" s="8" t="n">
         <v>81698096</v>
       </c>
-      <c r="C38" s="10" t="n">
+      <c r="C38" s="9" t="n">
         <v>589596394</v>
       </c>
     </row>
@@ -20852,7 +20852,7 @@
       <c r="B39" s="8" t="n">
         <v>81983304</v>
       </c>
-      <c r="C39" s="10" t="n">
+      <c r="C39" s="9" t="n">
         <v>609820455</v>
       </c>
     </row>
@@ -20863,7 +20863,7 @@
       <c r="B40" s="8" t="n">
         <v>81997362</v>
       </c>
-      <c r="C40" s="10" t="n">
+      <c r="C40" s="9" t="n">
         <v>609660712</v>
       </c>
     </row>
@@ -20874,7 +20874,7 @@
       <c r="B41" s="8" t="n">
         <v>81393650</v>
       </c>
-      <c r="C41" s="10" t="n">
+      <c r="C41" s="9" t="n">
         <v>601750729</v>
       </c>
     </row>
@@ -20885,7 +20885,7 @@
       <c r="B42" s="8" t="n">
         <v>81071314</v>
       </c>
-      <c r="C42" s="10" t="n">
+      <c r="C42" s="9" t="n">
         <v>748384539</v>
       </c>
     </row>
@@ -20896,7 +20896,7 @@
       <c r="B43" s="8" t="n">
         <v>82905275</v>
       </c>
-      <c r="C43" s="10" t="n">
+      <c r="C43" s="9" t="n">
         <v>669853633</v>
       </c>
     </row>
@@ -20907,7 +20907,7 @@
       <c r="B44" s="8" t="n">
         <v>82892486</v>
       </c>
-      <c r="C44" s="10" t="n">
+      <c r="C44" s="9" t="n">
         <v>881363303</v>
       </c>
     </row>
@@ -20918,7 +20918,7 @@
       <c r="B45" s="8" t="n">
         <v>81392598</v>
       </c>
-      <c r="C45" s="10" t="n">
+      <c r="C45" s="9" t="n">
         <v>616652515</v>
       </c>
     </row>
@@ -20929,7 +20929,7 @@
       <c r="B46" s="8" t="n">
         <v>80780600</v>
       </c>
-      <c r="C46" s="10" t="n">
+      <c r="C46" s="9" t="n">
         <v>721462100</v>
       </c>
     </row>
@@ -20982,7 +20982,7 @@
       <c r="B4" s="8" t="n">
         <v>22260418</v>
       </c>
-      <c r="C4" s="16" t="n">
+      <c r="C4" s="15" t="n">
         <v>199126653</v>
       </c>
     </row>
@@ -20993,7 +20993,7 @@
       <c r="B5" s="8" t="n">
         <v>20049103</v>
       </c>
-      <c r="C5" s="16" t="n">
+      <c r="C5" s="15" t="n">
         <v>199288073</v>
       </c>
     </row>
@@ -21004,7 +21004,7 @@
       <c r="B6" s="8" t="n">
         <v>19608500</v>
       </c>
-      <c r="C6" s="16" t="n">
+      <c r="C6" s="15" t="n">
         <v>199371413</v>
       </c>
     </row>
@@ -21015,7 +21015,7 @@
       <c r="B7" s="8" t="n">
         <v>20694080</v>
       </c>
-      <c r="C7" s="16" t="n">
+      <c r="C7" s="15" t="n">
         <v>201130293</v>
       </c>
     </row>
@@ -21026,7 +21026,7 @@
       <c r="B8" s="8" t="n">
         <v>20047045</v>
       </c>
-      <c r="C8" s="16" t="n">
+      <c r="C8" s="15" t="n">
         <v>201047791</v>
       </c>
     </row>
@@ -21037,7 +21037,7 @@
       <c r="B9" s="8" t="n">
         <v>19827687</v>
       </c>
-      <c r="C9" s="16" t="n">
+      <c r="C9" s="15" t="n">
         <v>198959637</v>
       </c>
     </row>
@@ -21048,7 +21048,7 @@
       <c r="B10" s="8" t="n">
         <v>22210445</v>
       </c>
-      <c r="C10" s="16" t="n">
+      <c r="C10" s="15" t="n">
         <v>199876056</v>
       </c>
     </row>
@@ -21059,7 +21059,7 @@
       <c r="B11" s="8" t="n">
         <v>22290963</v>
       </c>
-      <c r="C11" s="16" t="n">
+      <c r="C11" s="15" t="n">
         <v>201050169</v>
       </c>
     </row>
@@ -21070,7 +21070,7 @@
       <c r="B12" s="8" t="n">
         <v>20451094</v>
       </c>
-      <c r="C12" s="16" t="n">
+      <c r="C12" s="15" t="n">
         <v>200614168</v>
       </c>
     </row>
@@ -21081,7 +21081,7 @@
       <c r="B13" s="8" t="n">
         <v>20989720</v>
       </c>
-      <c r="C13" s="16" t="n">
+      <c r="C13" s="15" t="n">
         <v>199486549</v>
       </c>
     </row>
@@ -21092,7 +21092,7 @@
       <c r="B14" s="8" t="n">
         <v>5308717</v>
       </c>
-      <c r="C14" s="16" t="n">
+      <c r="C14" s="15" t="n">
         <v>199102932</v>
       </c>
     </row>
@@ -21103,7 +21103,7 @@
       <c r="B15" s="8" t="n">
         <v>3047232</v>
       </c>
-      <c r="C15" s="16" t="n">
+      <c r="C15" s="15" t="n">
         <v>199324786</v>
       </c>
     </row>
@@ -21114,7 +21114,7 @@
       <c r="B16" s="8" t="n">
         <v>5441675</v>
       </c>
-      <c r="C16" s="16" t="n">
+      <c r="C16" s="15" t="n">
         <v>199321246</v>
       </c>
     </row>
@@ -21125,7 +21125,7 @@
       <c r="B17" s="8" t="n">
         <v>4407165</v>
       </c>
-      <c r="C17" s="16" t="n">
+      <c r="C17" s="15" t="n">
         <v>201175722</v>
       </c>
     </row>
@@ -21136,7 +21136,7 @@
       <c r="B18" s="8" t="n">
         <v>4775800</v>
       </c>
-      <c r="C18" s="16" t="n">
+      <c r="C18" s="15" t="n">
         <v>201066857</v>
       </c>
     </row>
@@ -21147,7 +21147,7 @@
       <c r="B19" s="8" t="n">
         <v>342998</v>
       </c>
-      <c r="C19" s="16" t="n">
+      <c r="C19" s="15" t="n">
         <v>199090559</v>
       </c>
     </row>
@@ -21158,7 +21158,7 @@
       <c r="B20" s="8" t="n">
         <v>224706</v>
       </c>
-      <c r="C20" s="16" t="n">
+      <c r="C20" s="15" t="n">
         <v>199292376</v>
       </c>
     </row>
@@ -21169,7 +21169,7 @@
       <c r="B21" s="8" t="n">
         <v>43650</v>
       </c>
-      <c r="C21" s="16" t="n">
+      <c r="C21" s="15" t="n">
         <v>199351204</v>
       </c>
     </row>
@@ -21180,7 +21180,7 @@
       <c r="B22" s="8" t="n">
         <v>441162</v>
       </c>
-      <c r="C22" s="16" t="n">
+      <c r="C22" s="15" t="n">
         <v>201184186</v>
       </c>
     </row>
@@ -21191,7 +21191,7 @@
       <c r="B23" s="8" t="n">
         <v>177879</v>
       </c>
-      <c r="C23" s="16" t="n">
+      <c r="C23" s="15" t="n">
         <v>201123383</v>
       </c>
     </row>
@@ -21213,7 +21213,7 @@
       <c r="B27" s="8" t="n">
         <v>13804237</v>
       </c>
-      <c r="C27" s="14" t="n">
+      <c r="C27" s="13" t="n">
         <v>117638487</v>
       </c>
     </row>
@@ -21224,7 +21224,7 @@
       <c r="B28" s="8" t="n">
         <v>13861370</v>
       </c>
-      <c r="C28" s="16" t="n">
+      <c r="C28" s="15" t="n">
         <v>132840790</v>
       </c>
     </row>
@@ -21235,7 +21235,7 @@
       <c r="B29" s="8" t="n">
         <v>13797761</v>
       </c>
-      <c r="C29" s="16" t="n">
+      <c r="C29" s="15" t="n">
         <v>119838342</v>
       </c>
     </row>
@@ -21246,7 +21246,7 @@
       <c r="B30" s="8" t="n">
         <v>13808397</v>
       </c>
-      <c r="C30" s="16" t="n">
+      <c r="C30" s="15" t="n">
         <v>150513176</v>
       </c>
     </row>
@@ -21257,7 +21257,7 @@
       <c r="B31" s="8" t="n">
         <v>13744302</v>
       </c>
-      <c r="C31" s="16" t="n">
+      <c r="C31" s="15" t="n">
         <v>115966768</v>
       </c>
     </row>
@@ -21268,7 +21268,7 @@
       <c r="B32" s="8" t="n">
         <v>13912169</v>
       </c>
-      <c r="C32" s="16" t="n">
+      <c r="C32" s="15" t="n">
         <v>433191195</v>
       </c>
     </row>
@@ -21279,7 +21279,7 @@
       <c r="B33" s="8" t="n">
         <v>13742022</v>
       </c>
-      <c r="C33" s="16" t="n">
+      <c r="C33" s="15" t="n">
         <v>160335384</v>
       </c>
     </row>
@@ -21290,7 +21290,7 @@
       <c r="B34" s="8" t="n">
         <v>13796112</v>
       </c>
-      <c r="C34" s="16" t="n">
+      <c r="C34" s="15" t="n">
         <v>108301120</v>
       </c>
     </row>
@@ -21301,7 +21301,7 @@
       <c r="B35" s="8" t="n">
         <v>13857526</v>
       </c>
-      <c r="C35" s="16" t="n">
+      <c r="C35" s="15" t="n">
         <v>175086630</v>
       </c>
     </row>
@@ -21312,7 +21312,7 @@
       <c r="B36" s="8" t="n">
         <v>13798650</v>
       </c>
-      <c r="C36" s="16" t="n">
+      <c r="C36" s="15" t="n">
         <v>105033635</v>
       </c>
     </row>
@@ -21323,7 +21323,7 @@
       <c r="B37" s="8" t="n">
         <v>13812212</v>
       </c>
-      <c r="C37" s="16" t="n">
+      <c r="C37" s="15" t="n">
         <v>931231263</v>
       </c>
     </row>
@@ -21334,7 +21334,7 @@
       <c r="B38" s="8" t="n">
         <v>13800638</v>
       </c>
-      <c r="C38" s="16" t="n">
+      <c r="C38" s="15" t="n">
         <v>157665218</v>
       </c>
     </row>
@@ -21345,7 +21345,7 @@
       <c r="B39" s="8" t="n">
         <v>13860271</v>
       </c>
-      <c r="C39" s="16" t="n">
+      <c r="C39" s="15" t="n">
         <v>120801641</v>
       </c>
     </row>
@@ -21356,7 +21356,7 @@
       <c r="B40" s="8" t="n">
         <v>13801620</v>
       </c>
-      <c r="C40" s="16" t="n">
+      <c r="C40" s="15" t="n">
         <v>256547769</v>
       </c>
     </row>
@@ -21367,7 +21367,7 @@
       <c r="B41" s="8" t="n">
         <v>13867859</v>
       </c>
-      <c r="C41" s="16" t="n">
+      <c r="C41" s="15" t="n">
         <v>130335158</v>
       </c>
     </row>
@@ -21378,7 +21378,7 @@
       <c r="B42" s="8" t="n">
         <v>13855957</v>
       </c>
-      <c r="C42" s="16" t="n">
+      <c r="C42" s="15" t="n">
         <v>148617661</v>
       </c>
     </row>
@@ -21389,7 +21389,7 @@
       <c r="B43" s="8" t="n">
         <v>13813977</v>
       </c>
-      <c r="C43" s="16" t="n">
+      <c r="C43" s="15" t="n">
         <v>339858259</v>
       </c>
     </row>
@@ -21400,7 +21400,7 @@
       <c r="B44" s="8" t="n">
         <v>13871943</v>
       </c>
-      <c r="C44" s="16" t="n">
+      <c r="C44" s="15" t="n">
         <v>170647805</v>
       </c>
     </row>
@@ -21411,7 +21411,7 @@
       <c r="B45" s="8" t="n">
         <v>13861198</v>
       </c>
-      <c r="C45" s="16" t="n">
+      <c r="C45" s="15" t="n">
         <v>118565721</v>
       </c>
     </row>
@@ -21422,7 +21422,7 @@
       <c r="B46" s="8" t="n">
         <v>13865520</v>
       </c>
-      <c r="C46" s="16" t="n">
+      <c r="C46" s="15" t="n">
         <v>182291801</v>
       </c>
     </row>

</xml_diff>